<commit_message>
Corrección lógica de informe completo para incluir las compras/ventas IF
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20240903/20240903_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20240903/20240903_informe_completo_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ORO</t>
+          <t>ORO BLANCO</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -582,20 +582,20 @@
         <v>45538</v>
       </c>
       <c r="D4" t="n">
-        <v>16420.42</v>
+        <v>0.461</v>
       </c>
       <c r="E4" t="n">
-        <v>71</v>
+        <v>750000000</v>
       </c>
       <c r="F4" t="n">
-        <v>1165850</v>
+        <v>749769600</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>CFINHRFLA</t>
+          <t>BNPDBC050924</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -622,28 +622,68 @@
         <v>45538</v>
       </c>
       <c r="D5" t="n">
-        <v>15864.41</v>
+        <v>16420.42</v>
       </c>
       <c r="E5" t="n">
-        <v>4971</v>
+        <v>71</v>
       </c>
       <c r="F5" t="n">
-        <v>78861982</v>
+        <v>1165850</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>CFINHRFLA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45538</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45538</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15864.41</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4971</v>
+      </c>
+      <c r="F6" t="n">
+        <v>78861982</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>CFINHRFLB</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>COMPRA</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>RENTA VARIABLE</t>
         </is>

</xml_diff>